<commit_message>
Updated Hardware section to include Large Cable Transmission System, Added in Publication Experimental Data
</commit_message>
<xml_diff>
--- a/Hardware/Bowden_Transmission/Bill_of_Materials_AK60V1_1.xlsx
+++ b/Hardware/Bowden_Transmission/Bill_of_Materials_AK60V1_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Biomech_Lab\Jack_W\Exoskeleton_Design_Paper\Documentation\Bowden_Transmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EC478B-93FE-4285-A33A-1E23B2AE4417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5421614B-56CA-4804-AAC8-2AA25275C66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Item</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>Chain (1ft)</t>
-  </si>
-  <si>
     <t>TMotors AK60V1.1 KV80</t>
   </si>
   <si>
@@ -144,6 +141,15 @@
   </si>
   <si>
     <t>Cable Crimps (pack of 50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 04B Chain (1ft)</t>
+  </si>
+  <si>
+    <t>Bowden Tube</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Jagwire-Sport-Housing-Slick-Lube-Titanium/dp/B085NBZMJS/ref=sr_1_1?crid=1A5WX5ADQYM0Y&amp;dib=eyJ2IjoiMSJ9.CWV7EelBoN67bHKqG_VMGaAHwKq3lWAqkaCYopLdT43GyH4CDNeyWoQ_bFV_YrbZmhmwmsofP69GRzCCWYW_ULIkinZgZrdky8EGo_FPRa2GDLIPcrjwSu8T1nDFsZ03wyuLLatilRsdmpFkqvecV8S7AOhy1XjGVW6Ztcl1kgVL4_2zjOWbooP9z_kj4elJxdrMd7yL-uhr5ZcYm6F_Z725qnNy_c0-wNfaDt_xxhvLSabJzp2Ta9HzGpozVxtWGMo89NRT0qD_9iY1NxHHBedJp86w9TXZ0OfMm9s45WQ.7sQYhAOJzDOGkHvrSoGgv6F0CIzum6_7bjb1Zjv8zzc&amp;dib_tag=se&amp;keywords=Jagwire+Brake+Housing+CGX-SL+Slick-Lube+5+mm+%2810+m%29&amp;qid=1726249759&amp;s=sporting-goods&amp;sprefix=jagwire+brake+housing+cgx-sl+slick-lube+5+mm+10+m+%2Csporting%2C99&amp;sr=1-1</t>
   </si>
 </sst>
 </file>
@@ -240,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,6 +274,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:E11"/>
+      <selection activeCell="A20" sqref="A20:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +604,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -637,9 +646,9 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2">
@@ -655,10 +664,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -691,7 +700,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
@@ -709,10 +718,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -870,6 +879,20 @@
       <c r="E19" s="3">
         <f>SUM(E2:E18)</f>
         <v>1223.44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10">
+        <v>61.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>